<commit_message>
Cambios en nombres de las categorias utilizadas para las gráficas
</commit_message>
<xml_diff>
--- a/FILE.xlsx
+++ b/FILE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\50662\Desktop\Eléctrica\2023 II Semestre\Programación\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\50662\Desktop\Eléctrica\2023 II Semestre\Programación\Python\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,28 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Annual Budget</t>
-  </si>
-  <si>
-    <t>Annual Expense</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>Entertainment</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Feeding</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Months</t>
   </si>
@@ -87,16 +66,40 @@
     <t>December</t>
   </si>
   <si>
-    <t>Rent</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>Extra Income</t>
-  </si>
-  <si>
-    <t>Micelane</t>
+    <t>Salario</t>
+  </si>
+  <si>
+    <t>Comisiones</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>Otros Ingresos</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Domicilio</t>
+  </si>
+  <si>
+    <t>Entretenimiento</t>
+  </si>
+  <si>
+    <t>Servicios</t>
+  </si>
+  <si>
+    <t>Higiene</t>
+  </si>
+  <si>
+    <t>Seguros</t>
+  </si>
+  <si>
+    <t>Deudas</t>
+  </si>
+  <si>
+    <t>Transporte</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,47 +435,50 @@
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>250000</v>
@@ -507,10 +513,13 @@
       <c r="L2" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="1">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>250000</v>
@@ -545,10 +554,13 @@
       <c r="L3" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>250000</v>
@@ -583,10 +595,13 @@
       <c r="L4" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>250000</v>
@@ -621,10 +636,13 @@
       <c r="L5" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>250000</v>
@@ -659,10 +677,13 @@
       <c r="L6" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>250000</v>
@@ -697,10 +718,13 @@
       <c r="L7" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>250000</v>
@@ -735,10 +759,13 @@
       <c r="L8" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>250000</v>
@@ -773,10 +800,13 @@
       <c r="L9" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>250000</v>
@@ -811,10 +841,13 @@
       <c r="L10" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>250000</v>
@@ -849,10 +882,13 @@
       <c r="L11" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>250000</v>
@@ -887,10 +923,13 @@
       <c r="L12" s="1">
         <v>80000</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>210000</v>
@@ -924,6 +963,9 @@
       </c>
       <c r="L13" s="1">
         <v>90000</v>
+      </c>
+      <c r="M13" s="1">
+        <v>24500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>